<commit_message>
Rename "Source" to "Collection Type"
See https://aptivate.kanbantool.com/b/437721-internews-hid-2018#27567021.
</commit_message>
<xml_diff>
--- a/internewshid/chn_spreadsheet/tests/test_files/master_kobo_single_item.xlsx
+++ b/internewshid/chn_spreadsheet/tests/test_files/master_kobo_single_item.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author/>
   </authors>
   <commentList>
     <comment ref="D2" authorId="0">
@@ -217,7 +217,7 @@
     <t xml:space="preserve">Ennumerator</t>
   </si>
   <si>
-    <t xml:space="preserve">Source</t>
+    <t xml:space="preserve">Collection Type</t>
   </si>
   <si>
     <t xml:space="preserve">2018-10-01T12:31:38.287+06</t>
@@ -449,24 +449,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1048576"/>
+  <dimension ref="A1:K65536"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="53.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.53"/>
   </cols>
   <sheetData>

</xml_diff>